<commit_message>
update ES2015 data import
</commit_message>
<xml_diff>
--- a/Inputs_data/MP2015/research-2015-mort-imp-scale-rates.xlsx
+++ b/Inputs_data/MP2015/research-2015-mort-imp-scale-rates.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\Retirement Plans\Scale MP-2015\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\RSF_NYCTRS\Inputs_data\MP2015\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40BFCE7-1B46-4B05-B3B2-EFB68D250284}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21255" windowHeight="8280"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Male" sheetId="1" r:id="rId1"/>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -130,8 +131,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,16 +460,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:CD105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection activeCell="CB84" sqref="CB84"/>
       <selection pane="topRight" activeCell="CB84" sqref="CB84"/>
       <selection pane="bottomLeft" activeCell="CB84" sqref="CB84"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25474,7 +25475,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CD105"/>
   <sheetViews>

</xml_diff>